<commit_message>
Added report with two Pie Charts. Modified DataIn to support multiple queries within a single report.
</commit_message>
<xml_diff>
--- a/templates/BarLineOverlay.xlsx
+++ b/templates/BarLineOverlay.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Cat 0</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Cat 3</t>
-  </si>
-  <si>
-    <t>Cat 4</t>
   </si>
   <si>
     <t>Sales</t>
@@ -134,7 +131,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -146,7 +143,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>BarLineOverlay!$A$2</c:f>
+              <c:f>BarLineOverlay!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -158,9 +155,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>BarLineOverlay!$B$1:$F$1</c:f>
+              <c:f>BarLineOverlay!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Cat 0</c:v>
                 </c:pt>
@@ -172,33 +169,27 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Cat 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Cat 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BarLineOverlay!$B$2:$F$2</c:f>
+              <c:f>BarLineOverlay!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -213,8 +204,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="345870720"/>
-        <c:axId val="345872256"/>
+        <c:axId val="347555712"/>
+        <c:axId val="347563136"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -224,7 +215,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BarLineOverlay!$A$3</c:f>
+              <c:f>BarLineOverlay!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -235,9 +226,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>BarLineOverlay!$B$1:$F$1</c:f>
+              <c:f>BarLineOverlay!$A$2:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Cat 0</c:v>
                 </c:pt>
@@ -249,21 +240,18 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Cat 3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Cat 4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BarLineOverlay!$B$3:$F$3</c:f>
+              <c:f>BarLineOverlay!$C$2:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>17</c:v>
@@ -273,9 +261,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -292,20 +277,21 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="345870720"/>
-        <c:axId val="345872256"/>
+        <c:axId val="347555712"/>
+        <c:axId val="347563136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="345870720"/>
+        <c:axId val="347555712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="345872256"/>
+        <c:crossAx val="347563136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -313,7 +299,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345872256"/>
+        <c:axId val="347563136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,7 +310,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="345870720"/>
+        <c:crossAx val="347555712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -350,16 +336,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -668,37 +654,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2">
         <v>8</v>
@@ -706,39 +681,42 @@
       <c r="C2">
         <v>13</v>
       </c>
-      <c r="D2">
-        <v>18</v>
-      </c>
-      <c r="E2">
-        <v>23</v>
-      </c>
-      <c r="F2">
-        <v>28</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <f xml:space="preserve"> MOD(B2+4,20)</f>
         <v>12</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:F3" si="0" xml:space="preserve"> MOD(C2+4,20)</f>
+        <f t="shared" ref="C3" si="0" xml:space="preserve"> MOD(C2+4,20)</f>
         <v>17</v>
       </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
+      <c r="B4">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <f xml:space="preserve"> MOD(B4+4,20)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <f xml:space="preserve"> MOD(B5+4,20)</f>
         <v>7</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>